<commit_message>
Release Update 2.0 lebih rapih
</commit_message>
<xml_diff>
--- a/data/permintaan_server.xlsx
+++ b/data/permintaan_server.xlsx
@@ -441,7 +441,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U4"/>
+  <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,10 +450,10 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="25.2" customWidth="1" min="1" max="1"/>
-    <col width="25.2" customWidth="1" min="2" max="2"/>
-    <col width="10.8" customWidth="1" min="3" max="3"/>
+    <col width="16.8" customWidth="1" min="2" max="2"/>
+    <col width="12" customWidth="1" min="3" max="3"/>
     <col width="24" customWidth="1" min="4" max="4"/>
-    <col width="26.4" customWidth="1" min="5" max="5"/>
+    <col width="21.6" customWidth="1" min="5" max="5"/>
     <col width="9.6" customWidth="1" min="6" max="6"/>
     <col width="15.6" customWidth="1" min="7" max="7"/>
     <col width="16.8" customWidth="1" min="8" max="8"/>
@@ -582,7 +582,7 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>2025-05-20 11:48:05</t>
+          <t>2025-05-20 16:48:50</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
@@ -681,40 +681,42 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>2025-05-20 11:49:24</t>
+          <t>2025-05-20 16:53:45</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
-          <t>Muhamad Ferdiansyah</t>
-        </is>
-      </c>
-      <c r="C3" s="3" t="n">
-        <v>9281932</v>
+          <t>ayaka</t>
+        </is>
+      </c>
+      <c r="C3" s="3" t="inlineStr">
+        <is>
+          <t>27713123</t>
+        </is>
       </c>
       <c r="D3" s="3" t="inlineStr">
         <is>
-          <t>2025-05-01</t>
+          <t>2025-05-02</t>
         </is>
       </c>
       <c r="E3" s="3" t="inlineStr">
         <is>
-          <t>elder.ring@gmail.com</t>
+          <t>ayaka@hooy.co.id</t>
         </is>
       </c>
       <c r="F3" s="3" t="inlineStr">
         <is>
-          <t>ELI</t>
+          <t>INZ</t>
         </is>
       </c>
       <c r="G3" s="3" t="inlineStr">
         <is>
-          <t>IAC</t>
+          <t>TY</t>
         </is>
       </c>
       <c r="H3" s="3" t="inlineStr">
         <is>
-          <t>3 Bulan</t>
+          <t>1 Tahun</t>
         </is>
       </c>
       <c r="I3" s="3" t="inlineStr">
@@ -724,36 +726,42 @@
       </c>
       <c r="J3" s="3" t="inlineStr">
         <is>
-          <t>Development</t>
+          <t>Testing</t>
         </is>
       </c>
       <c r="K3" s="3" t="inlineStr">
         <is>
-          <t>Container</t>
+          <t>Physical Server</t>
         </is>
       </c>
       <c r="L3" s="3" t="inlineStr">
         <is>
-          <t>No Name</t>
+          <t>terserah</t>
         </is>
       </c>
       <c r="M3" s="3" t="inlineStr">
         <is>
-          <t>js</t>
-        </is>
-      </c>
-      <c r="N3" s="3" t="n">
-        <v>12</v>
-      </c>
-      <c r="O3" s="3" t="n">
-        <v>8</v>
-      </c>
-      <c r="P3" s="3" t="n">
-        <v>50</v>
+          <t>terserah</t>
+        </is>
+      </c>
+      <c r="N3" s="3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="O3" s="3" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="P3" s="3" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
       </c>
       <c r="Q3" s="3" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="R3" s="3" t="inlineStr">
@@ -763,124 +771,13 @@
       </c>
       <c r="S3" s="3" t="inlineStr">
         <is>
-          <t>ZIA</t>
-        </is>
-      </c>
-      <c r="T3" s="3" t="inlineStr">
-        <is>
-          <t>WEBEDC01</t>
-        </is>
-      </c>
+          <t>ZIB</t>
+        </is>
+      </c>
+      <c r="T3" s="3" t="inlineStr"/>
       <c r="U3" s="3" t="inlineStr">
         <is>
-          <t>ZIAWEBEDC01</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="3" t="inlineStr">
-        <is>
-          <t>2025-05-20 11:50:00</t>
-        </is>
-      </c>
-      <c r="B4" s="3" t="inlineStr">
-        <is>
-          <t>Aditya</t>
-        </is>
-      </c>
-      <c r="C4" s="3" t="inlineStr">
-        <is>
-          <t>9281932</t>
-        </is>
-      </c>
-      <c r="D4" s="3" t="inlineStr">
-        <is>
-          <t>2025-05-01</t>
-        </is>
-      </c>
-      <c r="E4" s="3" t="inlineStr">
-        <is>
-          <t>elder.ring@gmail.com</t>
-        </is>
-      </c>
-      <c r="F4" s="3" t="inlineStr">
-        <is>
-          <t>ELI</t>
-        </is>
-      </c>
-      <c r="G4" s="3" t="inlineStr">
-        <is>
-          <t>IAC</t>
-        </is>
-      </c>
-      <c r="H4" s="3" t="inlineStr">
-        <is>
-          <t>3 Bulan</t>
-        </is>
-      </c>
-      <c r="I4" s="3" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
-      <c r="J4" s="3" t="inlineStr">
-        <is>
-          <t>Development</t>
-        </is>
-      </c>
-      <c r="K4" s="3" t="inlineStr">
-        <is>
-          <t>Virtual Machine</t>
-        </is>
-      </c>
-      <c r="L4" s="3" t="inlineStr">
-        <is>
-          <t>No Name</t>
-        </is>
-      </c>
-      <c r="M4" s="3" t="inlineStr">
-        <is>
-          <t>js</t>
-        </is>
-      </c>
-      <c r="N4" s="3" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="O4" s="3" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="P4" s="3" t="inlineStr">
-        <is>
-          <t>50</t>
-        </is>
-      </c>
-      <c r="Q4" s="3" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="R4" s="3" t="inlineStr">
-        <is>
-          <t>Linux</t>
-        </is>
-      </c>
-      <c r="S4" s="3" t="inlineStr">
-        <is>
-          <t>UIB</t>
-        </is>
-      </c>
-      <c r="T4" s="3" t="inlineStr">
-        <is>
-          <t>APPEDC12</t>
-        </is>
-      </c>
-      <c r="U4" s="3" t="inlineStr">
-        <is>
-          <t>UIBAPPEDC12</t>
+          <t>ZIBPRTGRTG10</t>
         </is>
       </c>
     </row>

</xml_diff>